<commit_message>
Sidenav Fix, Seeder Fix
</commit_message>
<xml_diff>
--- a/public/uploads/Student Form.xlsx
+++ b/public/uploads/Student Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuuzen\Desktop\Oikos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA6D7AD-64C2-4C7C-8E57-6B1EFE23C2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A0B914-1F66-42C6-B58F-C8D63B9E249C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{909E23F8-EB81-4DD6-8013-332378BCD858}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
-  <si>
-    <t>Noob</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Enrolled</t>
   </si>
@@ -42,9 +39,6 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Mars</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>enroll_status</t>
   </si>
   <si>
-    <t>bday</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -178,6 +169,27 @@
   </si>
   <si>
     <t>Russian boy</t>
+  </si>
+  <si>
+    <t>ruby</t>
+  </si>
+  <si>
+    <t>humility</t>
+  </si>
+  <si>
+    <t>lapu-lapu</t>
+  </si>
+  <si>
+    <t>bday (YEAR-DATE-MONTH)</t>
+  </si>
+  <si>
+    <t>2024-07-02</t>
+  </si>
+  <si>
+    <t>2024-05-03</t>
+  </si>
+  <si>
+    <t>2024-26-01</t>
   </si>
 </sst>
 </file>
@@ -228,17 +240,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4158E3-35A6-44A2-8561-6866AC8C6EDE}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,240 +580,239 @@
     <col min="6" max="6" width="31.21875" customWidth="1"/>
     <col min="7" max="7" width="31.109375" customWidth="1"/>
     <col min="8" max="8" width="31" customWidth="1"/>
-    <col min="9" max="9" width="31.21875" customWidth="1"/>
+    <col min="9" max="9" width="31.21875" style="4" customWidth="1"/>
     <col min="10" max="10" width="31.109375" customWidth="1"/>
     <col min="11" max="11" width="31.21875" customWidth="1"/>
     <col min="12" max="12" width="30.88671875" customWidth="1"/>
     <col min="13" max="15" width="31.109375" customWidth="1"/>
     <col min="16" max="16" width="31" customWidth="1"/>
     <col min="17" max="17" width="31.33203125" customWidth="1"/>
-    <col min="18" max="18" width="31.21875" style="5" customWidth="1"/>
-    <col min="19" max="19" width="31.21875" customWidth="1"/>
+    <col min="18" max="19" width="31.21875" customWidth="1"/>
     <col min="20" max="22" width="31.109375" customWidth="1"/>
     <col min="23" max="23" width="31.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="3">
-        <v>45329</v>
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="J2">
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N2">
         <v>1246</v>
       </c>
       <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" t="s">
-        <v>3</v>
-      </c>
       <c r="Q2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="5">
+        <v>30</v>
+      </c>
+      <c r="R2">
         <v>132515</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2">
         <v>1345134</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
       </c>
       <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>45356</v>
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="J3">
         <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N3">
         <v>2345</v>
       </c>
       <c r="O3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R3" s="5">
+        <v>3</v>
+      </c>
+      <c r="R3">
         <v>12345</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3">
         <v>1234</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>45317</v>
+      <c r="I4" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="J4">
         <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N4">
         <v>13123</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R4" s="5">
+        <v>3</v>
+      </c>
+      <c r="R4">
         <v>1235</v>
       </c>
       <c r="S4">

</xml_diff>